<commit_message>
Screenshot folder modified. Test Cases Added. Test Data made dynamic
</commit_message>
<xml_diff>
--- a/MemberDues2.0/TestData/Data.xlsx
+++ b/MemberDues2.0/TestData/Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anik\eclipse-workspace\MemberDues2.0\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anik\git\Dues2TestFramework\MemberDues2.0\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35149116-F1D7-4C1D-85FA-45CB3D188A6F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F2FD3F0-190F-42DE-996D-62E29F4B5EC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>test123</t>
   </si>
@@ -34,16 +34,85 @@
   </si>
   <si>
     <t>123</t>
+  </si>
+  <si>
+    <t>Test Case Name</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Token</t>
+  </si>
+  <si>
+    <t>Login_to_Member_Portal</t>
+  </si>
+  <si>
+    <t>Logout_of_Member_Portal</t>
+  </si>
+  <si>
+    <t>ResetHeader</t>
+  </si>
+  <si>
+    <t>Member Security Questions</t>
+  </si>
+  <si>
+    <t>testuserd3432</t>
+  </si>
+  <si>
+    <t>tDuestest%3432</t>
+  </si>
+  <si>
+    <t>NewPassword</t>
+  </si>
+  <si>
+    <t>Test123</t>
+  </si>
+  <si>
+    <t>First_Time_Reset_Password</t>
+  </si>
+  <si>
+    <t>Q1Ans</t>
+  </si>
+  <si>
+    <t>Q2Ans</t>
+  </si>
+  <si>
+    <t>Q2Val</t>
+  </si>
+  <si>
+    <t>Q1Val</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>Texas</t>
+  </si>
+  <si>
+    <t>436</t>
+  </si>
+  <si>
+    <t>439</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -352,26 +421,117 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="22.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D2" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
3 Test Cases Added
</commit_message>
<xml_diff>
--- a/MemberDues2.0/TestData/Data.xlsx
+++ b/MemberDues2.0/TestData/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anik\git\Dues2TestFramework\MemberDues2.0\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F2FD3F0-190F-42DE-996D-62E29F4B5EC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16E7F0D6-4EA1-46B9-BAE3-B006B025B00E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="37">
   <si>
     <t>test123</t>
   </si>
@@ -97,6 +97,45 @@
   </si>
   <si>
     <t>439</t>
+  </si>
+  <si>
+    <t>Login_Error_On_Wrong_Userid</t>
+  </si>
+  <si>
+    <t>Login_Error_On_Wrong_Password</t>
+  </si>
+  <si>
+    <t>Login_Error_On_Wrong_Token</t>
+  </si>
+  <si>
+    <t>Login_Error_On_AppAccess_Restricted</t>
+  </si>
+  <si>
+    <t>Login_Error_On_Member_LoginRestricted</t>
+  </si>
+  <si>
+    <t>Login_Error_On_Member_Deleted</t>
+  </si>
+  <si>
+    <t>Login_Error_On_No_Data</t>
+  </si>
+  <si>
+    <t>1234</t>
+  </si>
+  <si>
+    <t>ExpectedError</t>
+  </si>
+  <si>
+    <t>Token authentication failure.</t>
+  </si>
+  <si>
+    <t>XT131</t>
+  </si>
+  <si>
+    <t>ERROR: Incorrect credentials.</t>
+  </si>
+  <si>
+    <t>test1234</t>
   </si>
 </sst>
 </file>
@@ -421,23 +460,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.85546875" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" customWidth="1"/>
     <col min="6" max="6" width="22.140625" customWidth="1"/>
+    <col min="11" max="11" width="27.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -468,8 +508,11 @@
       <c r="J1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -483,7 +526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -497,35 +540,107 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1</v>
+      </c>
+      <c r="K5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>34</v>
+      </c>
+      <c r="K7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B11" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C11" t="s">
         <v>12</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D11" t="s">
         <v>1</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E11" t="s">
         <v>14</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F11" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H11" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J11" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Code - 19.10.2020
</commit_message>
<xml_diff>
--- a/MemberDues2.0/TestData/Data.xlsx
+++ b/MemberDues2.0/TestData/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anik\git\Dues2TestFramework\MemberDues2.0\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16E7F0D6-4EA1-46B9-BAE3-B006B025B00E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A45C5490-B362-4C21-B1C5-25521CA13342}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="45">
   <si>
     <t>test123</t>
   </si>
@@ -123,9 +123,6 @@
     <t>1234</t>
   </si>
   <si>
-    <t>ExpectedError</t>
-  </si>
-  <si>
     <t>Token authentication failure.</t>
   </si>
   <si>
@@ -136,6 +133,33 @@
   </si>
   <si>
     <t>test1234</t>
+  </si>
+  <si>
+    <t>Are you sure to reset the password and set the security questions?</t>
+  </si>
+  <si>
+    <t>ExpectedString</t>
+  </si>
+  <si>
+    <t>Your access to the Union has been restricted. Please contact the Union Office for further details.</t>
+  </si>
+  <si>
+    <t>Your login has been restricted. Please contact the Union Office for further details.</t>
+  </si>
+  <si>
+    <t>Your do not have access to this union. Please contact the Union Office for further details.</t>
+  </si>
+  <si>
+    <t>testk123</t>
+  </si>
+  <si>
+    <t>test13</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>testphilips1t3441</t>
   </si>
 </sst>
 </file>
@@ -463,7 +487,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,9 +496,10 @@
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" customWidth="1"/>
-    <col min="6" max="6" width="22.140625" customWidth="1"/>
-    <col min="11" max="11" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" customWidth="1"/>
+    <col min="7" max="7" width="22.140625" customWidth="1"/>
+    <col min="12" max="12" width="23" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -491,25 +516,25 @@
         <v>6</v>
       </c>
       <c r="E1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" t="s">
         <v>13</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>19</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>16</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>18</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>17</v>
-      </c>
-      <c r="K1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -551,7 +576,7 @@
         <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>2</v>
@@ -559,8 +584,8 @@
       <c r="D5" t="s">
         <v>1</v>
       </c>
-      <c r="K5" t="s">
-        <v>35</v>
+      <c r="E5" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -576,8 +601,8 @@
       <c r="D6" t="s">
         <v>1</v>
       </c>
-      <c r="K6" t="s">
-        <v>35</v>
+      <c r="E6" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -591,26 +616,62 @@
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
-      </c>
-      <c r="K7" t="s">
         <v>33</v>
+      </c>
+      <c r="E7" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>27</v>
       </c>
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>28</v>
       </c>
+      <c r="B9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>29</v>
       </c>
+      <c r="B10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -626,21 +687,24 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" t="s">
         <v>14</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="H11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>20</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="J11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated Code with Captcha Changes and Token Entry
</commit_message>
<xml_diff>
--- a/MemberDues2.0/TestData/Data.xlsx
+++ b/MemberDues2.0/TestData/Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anik\git\Dues2TestFramework\MemberDues2.0\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A45C5490-B362-4C21-B1C5-25521CA13342}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9861E594-7B01-4AAA-BD67-BB2457C11424}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,14 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="45">
   <si>
     <t>test123</t>
   </si>
   <si>
-    <t>XT13</t>
-  </si>
-  <si>
     <t>123</t>
   </si>
   <si>
@@ -160,6 +157,9 @@
   </si>
   <si>
     <t>testphilips1t3441</t>
+  </si>
+  <si>
+    <t>demo</t>
   </si>
 </sst>
 </file>
@@ -487,13 +487,13 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38.85546875" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
     <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1"/>
@@ -504,208 +504,211 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
       <c r="E1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" t="s">
         <v>16</v>
-      </c>
-      <c r="J1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>1</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>1</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" s="1"/>
+      <c r="D4" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="E5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
         <v>0</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D6" t="s">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="E6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
         <v>0</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="E8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" t="s">
         <v>42</v>
       </c>
-      <c r="C9" t="s">
-        <v>43</v>
-      </c>
       <c r="D9" t="s">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="E9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D10" t="s">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="E10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
         <v>11</v>
       </c>
-      <c r="C11" t="s">
-        <v>12</v>
-      </c>
       <c r="D11" t="s">
-        <v>1</v>
+        <v>44</v>
       </c>
       <c r="E11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" t="s">
+        <v>19</v>
+      </c>
+      <c r="J11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I11" t="s">
+      <c r="K11" t="s">
         <v>20</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K11" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>